<commit_message>
Changed probabilities and redid graphs
</commit_message>
<xml_diff>
--- a/A3/Results.xlsx
+++ b/A3/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -52,12 +52,15 @@
   <si>
     <t>No samples succeeded.</t>
   </si>
+  <si>
+    <t>No samples succeeded</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +97,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,7 +126,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,6 +137,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -267,31 +279,31 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
                   <c:pt idx="0">
-                    <c:v>0.0427172096466985</c:v>
+                    <c:v>0.0334350953340946</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0254268962292264</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0144875690714488</c:v>
+                    <c:v>0.0133796382013864</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00784812615898899</c:v>
+                    <c:v>0.00806435845396731</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00418981805810228</c:v>
+                    <c:v>0.00412708008645337</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0024189925837009</c:v>
+                    <c:v>0.00245691140353086</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.00132323174026683</c:v>
+                    <c:v>0.00133964592147686</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.000762096052895482</c:v>
+                    <c:v>0.00076623760384918</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.000418052212301619</c:v>
+                    <c:v>0.000417607272197291</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -303,31 +315,31 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
                   <c:pt idx="0">
-                    <c:v>0.0427172096466985</c:v>
+                    <c:v>0.0334350953340946</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0254268962292264</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0144875690714488</c:v>
+                    <c:v>0.0133796382013864</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00784812615898899</c:v>
+                    <c:v>0.00806435845396731</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00418981805810228</c:v>
+                    <c:v>0.00412708008645337</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0024189925837009</c:v>
+                    <c:v>0.00245691140353086</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.00132323174026683</c:v>
+                    <c:v>0.00133964592147686</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.000762096052895482</c:v>
+                    <c:v>0.00076623760384918</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.000418052212301619</c:v>
+                    <c:v>0.000417607272197291</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -389,31 +401,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0533333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.058</c:v>
+                  <c:v>0.049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0506666666666666</c:v>
+                  <c:v>0.0536666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.048</c:v>
+                  <c:v>0.0465</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.048</c:v>
+                  <c:v>0.0496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.04787</c:v>
+                  <c:v>0.04913</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0476233333333333</c:v>
+                  <c:v>0.04817</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.047776</c:v>
+                  <c:v>0.047669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -430,11 +442,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2069446400"/>
-        <c:axId val="-2069813712"/>
+        <c:axId val="-2089935728"/>
+        <c:axId val="-2089932256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2069446400"/>
+        <c:axId val="-2089935728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -477,7 +489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069813712"/>
+        <c:crossAx val="-2089932256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -485,7 +497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2069813712"/>
+        <c:axId val="-2089932256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +548,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069446400"/>
+        <c:crossAx val="-2089935728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -700,31 +712,31 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
                   <c:pt idx="0">
-                    <c:v>0.236643191323984</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.147794398194347</c:v>
+                    <c:v>0.124096736459908</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0752946454073473</c:v>
+                    <c:v>0.0694694361119153</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0388742985422936</c:v>
+                    <c:v>0.041824778076111</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0220875562267328</c:v>
+                    <c:v>0.0208414556363004</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0123335663464517</c:v>
+                    <c:v>0.0125144222613924</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.00671109042125345</c:v>
+                    <c:v>0.0067214669133458</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00388524141068267</c:v>
+                    <c:v>0.00389618880097548</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.00213060433374165</c:v>
+                    <c:v>0.00213996826742367</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -736,31 +748,31 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
                   <c:pt idx="0">
-                    <c:v>0.236643191323984</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.147794398194347</c:v>
+                    <c:v>0.124096736459908</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0752946454073473</c:v>
+                    <c:v>0.0694694361119153</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0388742985422936</c:v>
+                    <c:v>0.041824778076111</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0220875562267328</c:v>
+                    <c:v>0.0208414556363004</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0123335663464517</c:v>
+                    <c:v>0.0125144222613924</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.00671109042125345</c:v>
+                    <c:v>0.0067214669133458</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00388524141068267</c:v>
+                    <c:v>0.00389618880097548</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.00213060433374165</c:v>
+                    <c:v>0.00213996826742367</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -822,31 +834,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.714285714285714</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.684210526315789</c:v>
+                  <c:v>0.785714285714285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.744186046511627</c:v>
+                  <c:v>0.767605633802816</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80759493670886</c:v>
+                  <c:v>0.754299754299754</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.781412639405204</c:v>
+                  <c:v>0.809838472834067</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.806443429731101</c:v>
+                  <c:v>0.797525877303711</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.808026604187136</c:v>
+                  <c:v>0.807131525270076</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.804090795709653</c:v>
+                  <c:v>0.804246881353379</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.804607463640121</c:v>
+                  <c:v>0.802516773475343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,11 +875,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2066328128"/>
-        <c:axId val="-2066702416"/>
+        <c:axId val="-2094230016"/>
+        <c:axId val="-2094226544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2066328128"/>
+        <c:axId val="-2094230016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +922,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066702416"/>
+        <c:crossAx val="-2094226544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -918,7 +930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2066702416"/>
+        <c:axId val="-2094226544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066328128"/>
+        <c:crossAx val="-2094230016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1137,32 +1149,29 @@
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.205322857944538</c:v>
+                    <c:v>0.210862426626848</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0692269217524892</c:v>
+                    <c:v>0.110842516162494</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0489508258118556</c:v>
+                    <c:v>0.0763424746160315</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0334163586076558</c:v>
+                    <c:v>0.0318372937617831</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0214980412022713</c:v>
+                    <c:v>0.0188144280110539</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0113847424241665</c:v>
+                    <c:v>0.0114864724017437</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00656754391770327</c:v>
+                    <c:v>0.00663761199611901</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.00364881664004688</c:v>
+                    <c:v>0.00357316515481106</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1173,32 +1182,29 @@
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
-                  <c:pt idx="0">
-                    <c:v>0.0</c:v>
-                  </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.205322857944538</c:v>
+                    <c:v>0.210862426626848</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0692269217524892</c:v>
+                    <c:v>0.110842516162494</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0489508258118556</c:v>
+                    <c:v>0.0763424746160315</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0334163586076558</c:v>
+                    <c:v>0.0318372937617831</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0214980412022713</c:v>
+                    <c:v>0.0188144280110539</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0113847424241665</c:v>
+                    <c:v>0.0114864724017437</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00656754391770327</c:v>
+                    <c:v>0.00663761199611901</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.00364881664004688</c:v>
+                    <c:v>0.00357316515481106</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1259,32 +1265,29 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.111111111111111</c:v>
+                  <c:v>0.166666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0512820512820512</c:v>
+                  <c:v>0.103448275862068</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0512820512820512</c:v>
+                  <c:v>0.139240506329113</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0855018587360594</c:v>
+                  <c:v>0.0866666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.108343711083437</c:v>
+                  <c:v>0.0820073439412484</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.101626016260162</c:v>
+                  <c:v>0.100795755968169</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10062034739454</c:v>
+                  <c:v>0.101558572146807</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.102364877607211</c:v>
+                  <c:v>0.098722545943523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1301,11 +1304,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2066899344"/>
-        <c:axId val="-2029707008"/>
+        <c:axId val="-2094195952"/>
+        <c:axId val="-2094192480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2066899344"/>
+        <c:axId val="-2094195952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,7 +1351,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2029707008"/>
+        <c:crossAx val="-2094192480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1356,7 +1359,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029707008"/>
+        <c:axId val="-2094192480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,7 +1410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066899344"/>
+        <c:crossAx val="-2094195952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1575,26 +1578,29 @@
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>0.692964645562816</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.335480066471914</c:v>
+                    <c:v>0.33466401061363</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.179256188657016</c:v>
+                    <c:v>0.199457141126969</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.11766797686705</c:v>
+                    <c:v>0.108634226650719</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0569130518536776</c:v>
+                    <c:v>0.060571459695006</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.0343796485621206</c:v>
+                    <c:v>0.0343923512578334</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.0185565034308201</c:v>
+                    <c:v>0.0185973684856253</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1605,26 +1611,29 @@
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>0.692964645562816</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.335480066471914</c:v>
+                    <c:v>0.33466401061363</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.179256188657016</c:v>
+                    <c:v>0.199457141126969</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.11766797686705</c:v>
+                    <c:v>0.108634226650719</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0569130518536776</c:v>
+                    <c:v>0.060571459695006</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.0343796485621206</c:v>
+                    <c:v>0.0343923512578334</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.0185565034308201</c:v>
+                    <c:v>0.0185973684856253</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1685,26 +1694,29 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.375</c:v>
+                  <c:v>0.285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.586206896551724</c:v>
+                  <c:v>0.608695652173913</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.463768115942029</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.464406779661016</c:v>
+                  <c:v>0.42578125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.422446406052963</c:v>
+                  <c:v>0.460966542750929</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.449837015574067</c:v>
+                  <c:v>0.4490538573508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,11 +1733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072386432"/>
-        <c:axId val="-2076316528"/>
+        <c:axId val="-2094163760"/>
+        <c:axId val="-2094160288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072386432"/>
+        <c:axId val="-2094163760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1768,7 +1780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076316528"/>
+        <c:crossAx val="-2094160288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1776,7 +1788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076316528"/>
+        <c:axId val="-2094160288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,7 +1839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072386432"/>
+        <c:crossAx val="-2094163760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4438,8 +4450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4486,10 +4498,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E7" s="1">
-        <v>4.2717209646698499E-2</v>
+        <v>3.3435095334094597E-2</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -4497,7 +4509,7 @@
         <v>300</v>
       </c>
       <c r="C8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>5.3333333333333302E-2</v>
@@ -4511,13 +4523,13 @@
         <v>1000</v>
       </c>
       <c r="C9" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1">
-        <v>5.8000000000000003E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>1.44875690714488E-2</v>
+        <v>1.33796382013864E-2</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
@@ -4525,13 +4537,13 @@
         <v>3000</v>
       </c>
       <c r="C10" s="1">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1">
-        <v>5.0666666666666603E-2</v>
+        <v>5.3666666666666599E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>7.8481261589889908E-3</v>
+        <v>8.0643584539673106E-3</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -4539,13 +4551,13 @@
         <v>10000</v>
       </c>
       <c r="C11" s="1">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="D11" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>4.65E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>4.1898180581022796E-3</v>
+        <v>4.1270800864533696E-3</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -4553,13 +4565,13 @@
         <v>30000</v>
       </c>
       <c r="C12" s="1">
-        <v>901</v>
+        <v>848</v>
       </c>
       <c r="D12" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>4.9599999999999998E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>2.4189925837009001E-3</v>
+        <v>2.4569114035308602E-3</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -4567,13 +4579,13 @@
         <v>100000</v>
       </c>
       <c r="C13" s="1">
-        <v>2882</v>
+        <v>2757</v>
       </c>
       <c r="D13" s="1">
-        <v>4.7870000000000003E-2</v>
+        <v>4.913E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>1.3232317402668301E-3</v>
+        <v>1.3396459214768601E-3</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -4581,13 +4593,13 @@
         <v>300000</v>
       </c>
       <c r="C14" s="1">
-        <v>9011</v>
+        <v>8627</v>
       </c>
       <c r="D14" s="1">
-        <v>4.7623333333333302E-2</v>
+        <v>4.8169999999999998E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>7.6209605289548202E-4</v>
+        <v>7.6623760384917998E-4</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -4595,16 +4607,61 @@
         <v>1000000</v>
       </c>
       <c r="C15" s="1">
-        <v>30111</v>
+        <v>28490</v>
       </c>
       <c r="D15" s="1">
-        <v>4.7775999999999999E-2</v>
+        <v>4.7669000000000003E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>4.1805221230161902E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+        <v>4.1760727219729098E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
@@ -4631,10 +4688,10 @@
         <v>3</v>
       </c>
       <c r="D34" s="1">
-        <v>0.71428571428571397</v>
+        <v>1</v>
       </c>
       <c r="E34" s="1">
-        <v>0.23664319132398401</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
@@ -4642,13 +4699,13 @@
         <v>300</v>
       </c>
       <c r="C35" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D35" s="1">
-        <v>0.68421052631578905</v>
+        <v>0.78571428571428503</v>
       </c>
       <c r="E35" s="1">
-        <v>0.147794398194347</v>
+        <v>0.124096736459908</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
@@ -4656,13 +4713,13 @@
         <v>1000</v>
       </c>
       <c r="C36" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" s="1">
-        <v>0.74418604651162701</v>
+        <v>0.76760563380281599</v>
       </c>
       <c r="E36" s="1">
-        <v>7.5294645407347302E-2</v>
+        <v>6.9469436111915306E-2</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
@@ -4670,13 +4727,13 @@
         <v>3000</v>
       </c>
       <c r="C37" s="1">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D37" s="1">
-        <v>0.80759493670885996</v>
+        <v>0.75429975429975404</v>
       </c>
       <c r="E37" s="1">
-        <v>3.88742985422936E-2</v>
+        <v>4.1824778076110999E-2</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
@@ -4684,13 +4741,13 @@
         <v>10000</v>
       </c>
       <c r="C38" s="1">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D38" s="1">
-        <v>0.781412639405204</v>
+        <v>0.80983847283406696</v>
       </c>
       <c r="E38" s="1">
-        <v>2.20875562267328E-2</v>
+        <v>2.08414556363004E-2</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
@@ -4698,13 +4755,13 @@
         <v>30000</v>
       </c>
       <c r="C39" s="1">
-        <v>849</v>
+        <v>828</v>
       </c>
       <c r="D39" s="1">
-        <v>0.80644342973110095</v>
+        <v>0.79752587730371105</v>
       </c>
       <c r="E39" s="1">
-        <v>1.23335663464517E-2</v>
+        <v>1.25144222613924E-2</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
@@ -4712,13 +4769,13 @@
         <v>100000</v>
       </c>
       <c r="C40" s="1">
-        <v>2749</v>
+        <v>2814</v>
       </c>
       <c r="D40" s="1">
-        <v>0.80802660418713601</v>
+        <v>0.80713152527007603</v>
       </c>
       <c r="E40" s="1">
-        <v>6.7110904212534499E-3</v>
+        <v>6.7214669133457998E-3</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
@@ -4726,13 +4783,13 @@
         <v>300000</v>
       </c>
       <c r="C41" s="1">
-        <v>8780</v>
+        <v>8336</v>
       </c>
       <c r="D41" s="1">
-        <v>0.80409079570965303</v>
+        <v>0.80424688135337896</v>
       </c>
       <c r="E41" s="1">
-        <v>3.8852414106826699E-3</v>
+        <v>3.89618880097548E-3</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
@@ -4740,14 +4797,29 @@
         <v>1000000</v>
       </c>
       <c r="C42" s="1">
-        <v>28970</v>
+        <v>27756</v>
       </c>
       <c r="D42" s="1">
-        <v>0.80460746364012103</v>
+        <v>0.802516773475343</v>
       </c>
       <c r="E42" s="1">
-        <v>2.1306043337416501E-3</v>
-      </c>
+        <v>2.1399682674236699E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
@@ -4772,126 +4844,122 @@
       <c r="B64" s="1">
         <v>100</v>
       </c>
-      <c r="C64" s="1">
-        <v>4</v>
-      </c>
-      <c r="D64" s="1">
-        <v>0</v>
-      </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
+      <c r="C64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <v>300</v>
       </c>
-      <c r="C65" s="1">
-        <v>9</v>
-      </c>
-      <c r="D65" s="1">
-        <v>0.11111111111111099</v>
-      </c>
-      <c r="E65" s="1">
-        <v>0.205322857944538</v>
+      <c r="C65" s="6">
+        <v>8</v>
+      </c>
+      <c r="D65" s="6">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="E65" s="6">
+        <v>0.21086242662684801</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="1">
         <v>1000</v>
       </c>
-      <c r="C66" s="1">
-        <v>27</v>
-      </c>
-      <c r="D66" s="1">
-        <v>5.1282051282051197E-2</v>
-      </c>
-      <c r="E66" s="1">
-        <v>6.9226921752489207E-2</v>
+      <c r="C66" s="6">
+        <v>26</v>
+      </c>
+      <c r="D66" s="6">
+        <v>0.10344827586206801</v>
+      </c>
+      <c r="E66" s="6">
+        <v>0.11084251616249401</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="1">
         <v>3000</v>
       </c>
-      <c r="C67" s="1">
-        <v>82</v>
-      </c>
-      <c r="D67" s="1">
-        <v>5.1282051282051197E-2</v>
-      </c>
-      <c r="E67" s="1">
-        <v>4.89508258118556E-2</v>
+      <c r="C67" s="6">
+        <v>83</v>
+      </c>
+      <c r="D67" s="6">
+        <v>0.139240506329113</v>
+      </c>
+      <c r="E67" s="6">
+        <v>7.6342474616031497E-2</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="1">
         <v>10000</v>
       </c>
-      <c r="C68" s="1">
-        <v>285</v>
-      </c>
-      <c r="D68" s="1">
-        <v>8.5501858736059394E-2</v>
-      </c>
-      <c r="E68" s="1">
-        <v>3.3416358607655801E-2</v>
+      <c r="C68" s="6">
+        <v>270</v>
+      </c>
+      <c r="D68" s="6">
+        <v>8.66666666666666E-2</v>
+      </c>
+      <c r="E68" s="6">
+        <v>3.1837293761783098E-2</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="1">
         <v>30000</v>
       </c>
-      <c r="C69" s="1">
-        <v>828</v>
-      </c>
-      <c r="D69" s="1">
-        <v>0.108343711083437</v>
-      </c>
-      <c r="E69" s="1">
-        <v>2.1498041202271299E-2</v>
+      <c r="C69" s="6">
+        <v>833</v>
+      </c>
+      <c r="D69" s="6">
+        <v>8.2007343941248395E-2</v>
+      </c>
+      <c r="E69" s="6">
+        <v>1.8814428011053898E-2</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="1">
         <v>100000</v>
       </c>
-      <c r="C70" s="1">
-        <v>2773</v>
-      </c>
-      <c r="D70" s="1">
-        <v>0.101626016260162</v>
-      </c>
-      <c r="E70" s="1">
-        <v>1.13847424241665E-2</v>
+      <c r="C70" s="6">
+        <v>2734</v>
+      </c>
+      <c r="D70" s="6">
+        <v>0.100795755968169</v>
+      </c>
+      <c r="E70" s="6">
+        <v>1.14864724017437E-2</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="1">
         <v>300000</v>
       </c>
-      <c r="C71" s="1">
-        <v>8382</v>
-      </c>
-      <c r="D71" s="1">
-        <v>0.10062034739454</v>
-      </c>
-      <c r="E71" s="1">
-        <v>6.5675439177032696E-3</v>
+      <c r="C71" s="6">
+        <v>8897</v>
+      </c>
+      <c r="D71" s="6">
+        <v>0.101558572146807</v>
+      </c>
+      <c r="E71" s="6">
+        <v>6.6376119961190101E-3</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="1">
         <v>1000000</v>
       </c>
-      <c r="C72" s="1">
-        <v>28859</v>
-      </c>
-      <c r="D72" s="1">
-        <v>0.102364877607211</v>
-      </c>
-      <c r="E72" s="1">
-        <v>3.6488166400468801E-3</v>
+      <c r="C72" s="6">
+        <v>30350</v>
+      </c>
+      <c r="D72" s="6">
+        <v>9.8722545943523005E-2</v>
+      </c>
+      <c r="E72" s="6">
+        <v>3.5731651548110599E-3</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
@@ -4917,17 +4985,21 @@
       <c r="B101" s="1">
         <v>100</v>
       </c>
-      <c r="C101" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
+      <c r="C101" s="1">
+        <v>3</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B102" s="1">
         <v>300</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D102" s="1"/>
@@ -4938,7 +5010,7 @@
         <v>1000</v>
       </c>
       <c r="C103" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D103" s="1">
         <v>0.5</v>
@@ -4952,13 +5024,13 @@
         <v>3000</v>
       </c>
       <c r="C104" s="1">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D104" s="1">
-        <v>0.375</v>
+        <v>0.28571428571428498</v>
       </c>
       <c r="E104" s="1">
-        <v>0.33548006647191397</v>
+        <v>0.33466401061362999</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.2">
@@ -4966,13 +5038,13 @@
         <v>10000</v>
       </c>
       <c r="C105" s="1">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D105" s="1">
-        <v>0.58620689655172398</v>
+        <v>0.60869565217391297</v>
       </c>
       <c r="E105" s="1">
-        <v>0.17925618865701601</v>
+        <v>0.199457141126969</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
@@ -4980,13 +5052,13 @@
         <v>30000</v>
       </c>
       <c r="C106" s="1">
-        <v>838</v>
+        <v>846</v>
       </c>
       <c r="D106" s="1">
-        <v>0.46376811594202899</v>
+        <v>0.36</v>
       </c>
       <c r="E106" s="1">
-        <v>0.11766797686704999</v>
+        <v>0.10863422665071901</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
@@ -4994,13 +5066,13 @@
         <v>100000</v>
       </c>
       <c r="C107" s="1">
-        <v>2852</v>
+        <v>2806</v>
       </c>
       <c r="D107" s="1">
-        <v>0.46440677966101601</v>
+        <v>0.42578125</v>
       </c>
       <c r="E107" s="1">
-        <v>5.69130518536776E-2</v>
+        <v>6.0571459695005998E-2</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
@@ -5008,13 +5080,13 @@
         <v>300000</v>
       </c>
       <c r="C108" s="1">
-        <v>8368</v>
+        <v>9170</v>
       </c>
       <c r="D108" s="1">
-        <v>0.42244640605296302</v>
+        <v>0.46096654275092902</v>
       </c>
       <c r="E108" s="1">
-        <v>3.4379648562120599E-2</v>
+        <v>3.4392351257833402E-2</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.2">
@@ -5022,13 +5094,13 @@
         <v>1000000</v>
       </c>
       <c r="C109" s="1">
-        <v>27732</v>
+        <v>29147</v>
       </c>
       <c r="D109" s="1">
-        <v>0.44983701557406702</v>
+        <v>0.4490538573508</v>
       </c>
       <c r="E109" s="1">
-        <v>1.85565034308201E-2</v>
+        <v>1.85973684856253E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>